<commit_message>
WIP: environmental swimming submodule
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="98">
   <si>
     <t>Variable</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Swimming</t>
   </si>
   <si>
-    <t>Tap water</t>
-  </si>
-  <si>
     <t>Misc</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t xml:space="preserve">T </t>
   </si>
   <si>
-    <t>P_sal</t>
-  </si>
-  <si>
     <t xml:space="preserve">Temperature of watershed water  </t>
   </si>
   <si>
@@ -216,6 +210,9 @@
     <t>day</t>
   </si>
   <si>
+    <t>O'Flaherty et al. (2019)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Time in river before arriving DWTP </t>
   </si>
   <si>
@@ -289,6 +286,48 @@
   </si>
   <si>
     <t>log10</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Volume of bathing site</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flowrate of river </t>
+  </si>
+  <si>
+    <t>m3/day</t>
+  </si>
+  <si>
+    <t>w_ingest.adult</t>
+  </si>
+  <si>
+    <t>w_ingest.child</t>
+  </si>
+  <si>
+    <t>swimmer_type</t>
+  </si>
+  <si>
+    <t>1 if adult or 0 if children</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Quantity of water ingested through an adult swimming for an hour</t>
+  </si>
+  <si>
+    <t>Quantity of water ingested through a child swimming for an hour</t>
+  </si>
+  <si>
+    <t>sal</t>
   </si>
 </sst>
 </file>
@@ -336,7 +375,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,12 +444,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -437,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -456,8 +489,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -781,23 +812,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.7265625" customWidth="1"/>
     <col min="2" max="2" width="11.08984375" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="49.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="59.6328125" customWidth="1"/>
     <col min="5" max="5" width="11.7265625" customWidth="1"/>
     <col min="6" max="6" width="14.7265625" customWidth="1"/>
     <col min="7" max="7" width="10.36328125" customWidth="1"/>
     <col min="8" max="9" width="9.54296875" customWidth="1"/>
-    <col min="10" max="10" width="8.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" customWidth="1"/>
     <col min="11" max="11" width="3.26953125" customWidth="1"/>
     <col min="12" max="12" width="5.6328125" customWidth="1"/>
     <col min="13" max="13" width="2.453125" customWidth="1"/>
@@ -860,12 +891,12 @@
       <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="20"/>
+      <c r="B2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
         <v>25</v>
@@ -887,9 +918,9 @@
       <c r="B3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
         <v>25</v>
@@ -909,23 +940,39 @@
         <v>34</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="H4" s="2">
+        <v>8640</v>
+      </c>
+      <c r="I4" s="2">
+        <v>172800</v>
+      </c>
+      <c r="J4" s="2">
+        <v>17280</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="O4" t="s">
+        <v>58</v>
+      </c>
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
@@ -935,125 +982,164 @@
       <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="2"/>
+      <c r="C5" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2">
+        <v>67500</v>
+      </c>
+      <c r="I5" s="2">
+        <v>82500</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="19"/>
+      <c r="O5" t="s">
+        <v>58</v>
+      </c>
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="A6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>70.67</v>
+      </c>
+      <c r="J6" s="3"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="3"/>
+      <c r="O6" t="s">
+        <v>58</v>
+      </c>
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="C7" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>205.33</v>
+      </c>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="3"/>
+      <c r="O7" t="s">
+        <v>58</v>
+      </c>
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
+      <c r="A8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="2">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="I8" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>45</v>
+      <c r="B9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>5</v>
@@ -1061,161 +1147,143 @@
       <c r="G9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="2">
-        <v>21</v>
-      </c>
-      <c r="I9" s="2">
-        <v>28</v>
-      </c>
-      <c r="J9" s="3"/>
+      <c r="H9" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="I9" s="3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" t="s">
-        <v>46</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>4</v>
+      <c r="B10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="2">
-        <v>17.32</v>
-      </c>
-      <c r="I10" s="3">
-        <v>25.38</v>
-      </c>
-      <c r="J10" s="3">
-        <v>22.73</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="L10" s="2">
+        <v>100</v>
+      </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="P10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="F11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <v>0.89</v>
+      </c>
+      <c r="I11">
+        <v>0.99</v>
+      </c>
+      <c r="J11">
+        <v>0.99</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="O11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.31</v>
-      </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" t="s">
-        <v>52</v>
-      </c>
-      <c r="P11" s="2" t="s">
+      <c r="B12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="F12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <v>0.1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="O12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I12" s="3">
-        <v>1</v>
-      </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" t="s">
-        <v>57</v>
-      </c>
-      <c r="P12" s="2" t="s">
+      <c r="B13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>5</v>
@@ -1223,212 +1291,208 @@
       <c r="G13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="I13" s="3">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="J13" s="2"/>
+      <c r="H13">
+        <v>0.18</v>
+      </c>
+      <c r="I13">
+        <v>0.97</v>
+      </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
       <c r="O13" t="s">
-        <v>80</v>
-      </c>
-      <c r="P13" s="2"/>
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="2">
-        <v>100</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="H14">
+        <v>0.49</v>
+      </c>
+      <c r="I14">
+        <v>0.99</v>
+      </c>
+      <c r="J14">
+        <v>0.99</v>
+      </c>
+      <c r="K14" s="2"/>
       <c r="O14" t="s">
-        <v>64</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H15">
-        <v>0.89</v>
+        <v>0.95</v>
       </c>
       <c r="I15">
         <v>0.99</v>
       </c>
-      <c r="J15">
-        <v>0.99</v>
-      </c>
       <c r="K15" s="2"/>
       <c r="O15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16">
+        <v>5.7</v>
+      </c>
+      <c r="I16">
+        <v>6.2</v>
+      </c>
+      <c r="O16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16">
-        <v>0.1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2"/>
-      <c r="O16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17">
+        <v>0.84</v>
+      </c>
+      <c r="I17">
+        <v>0.99</v>
+      </c>
+      <c r="J17">
+        <v>0.99</v>
+      </c>
+      <c r="O17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17">
-        <v>0.18</v>
-      </c>
-      <c r="I17">
-        <v>0.97</v>
-      </c>
-      <c r="K17" s="2"/>
-      <c r="O17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H18">
-        <v>0.49</v>
-      </c>
-      <c r="I18">
-        <v>0.99</v>
-      </c>
-      <c r="J18">
-        <v>0.99</v>
-      </c>
+      <c r="H18" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J18" s="3"/>
       <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
       <c r="O18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>83</v>
+        <v>35</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>5</v>
@@ -1436,109 +1500,167 @@
       <c r="G19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H19">
-        <v>0.95</v>
-      </c>
-      <c r="I19">
-        <v>0.99</v>
-      </c>
+      <c r="H19" s="2">
+        <v>21</v>
+      </c>
+      <c r="I19" s="2">
+        <v>28</v>
+      </c>
+      <c r="J19" s="3"/>
       <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
       <c r="O19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>84</v>
+        <v>35</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="2">
+        <v>17.32</v>
+      </c>
+      <c r="I20" s="3">
+        <v>25.38</v>
+      </c>
+      <c r="J20" s="3">
+        <v>22.73</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" t="s">
+        <v>46</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20">
-        <v>5.7</v>
-      </c>
-      <c r="I20">
-        <v>6.2</v>
-      </c>
-      <c r="O20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H21">
-        <v>0.84</v>
-      </c>
-      <c r="I21">
-        <v>0.99</v>
-      </c>
-      <c r="J21">
-        <v>0.99</v>
-      </c>
+      <c r="H21" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
       <c r="O21" t="s">
-        <v>80</v>
+        <v>50</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="721" yWindow="594" count="9">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K15:K19">
-      <formula1>I15</formula1>
-      <formula2>J15</formula2>
+  <dataValidations xWindow="721" yWindow="594" count="8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K11:K15">
+      <formula1>I11</formula1>
+      <formula2>J11</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L2:L6 L8:L13"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J2:J6 J8:J13">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L18:L22 L2:L9"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J18:J22 J2:J9">
       <formula1>H2</formula1>
       <formula2>I2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="L7">
-      <formula1>H7</formula1>
-      <formula2>I7</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M13"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N13"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K2:K13">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M18:M22 M2:M9"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N18:N22 N2:N9"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K18:K22 K2:K9">
       <formula1>I2</formula1>
       <formula2>J2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I13">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I18:I22 I2:I9">
       <formula1>H2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H13">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H18:H22 H2:H9">
       <formula1>I2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1547,17 +1669,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="721" yWindow="594" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
+          <x14:formula1>
+            <xm:f>ListItem!$A$2:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>F11:F22 F9 F2:F7</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Truncated" prompt="Is the probability distribution truncated?">
           <x14:formula1>
             <xm:f>ListItem!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G21</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
-          <x14:formula1>
-            <xm:f>ListItem!$A$2:$A$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F13 F15:F21</xm:sqref>
+          <xm:sqref>G2:G22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
environmental module first draft
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="119">
   <si>
     <t>Variable</t>
   </si>
@@ -328,6 +328,69 @@
   </si>
   <si>
     <t>sal</t>
+  </si>
+  <si>
+    <t>n_harvest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lettuce harvest time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attachment of water onto lettuce after sprinkler irrigation </t>
+  </si>
+  <si>
+    <t>w_attach</t>
+  </si>
+  <si>
+    <t>ml/g</t>
+  </si>
+  <si>
+    <t>Mok and Hamilton, (2014)</t>
+  </si>
+  <si>
+    <t>Used in lettuce model of O'Flaherty et al. (2019)</t>
+  </si>
+  <si>
+    <t>k1</t>
+  </si>
+  <si>
+    <t>k2</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Proportion of cells that have a fast decay</t>
+  </si>
+  <si>
+    <t>Rate constant for the cells with a slow decay</t>
+  </si>
+  <si>
+    <t>Rate constant for the cells with a fast decay</t>
+  </si>
+  <si>
+    <t>/day</t>
+  </si>
+  <si>
+    <t>McKellar et al. (2014)</t>
+  </si>
+  <si>
+    <t>r_wash</t>
+  </si>
+  <si>
+    <t>Rate of decay in consumer washing of lettuce</t>
+  </si>
+  <si>
+    <t>l_consum</t>
+  </si>
+  <si>
+    <t>Lettuce consumption</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>LogNormal3</t>
   </si>
 </sst>
 </file>
@@ -375,7 +438,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,12 +505,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -470,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -488,7 +545,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -812,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -829,10 +885,9 @@
     <col min="7" max="7" width="10.36328125" customWidth="1"/>
     <col min="8" max="9" width="9.54296875" customWidth="1"/>
     <col min="10" max="10" width="11.81640625" customWidth="1"/>
-    <col min="11" max="11" width="3.26953125" customWidth="1"/>
-    <col min="12" max="12" width="5.6328125" customWidth="1"/>
-    <col min="13" max="13" width="2.453125" customWidth="1"/>
-    <col min="14" max="14" width="2.54296875" customWidth="1"/>
+    <col min="11" max="12" width="6.90625" customWidth="1"/>
+    <col min="13" max="13" width="7.453125" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" customWidth="1"/>
     <col min="15" max="15" width="23.453125" customWidth="1"/>
     <col min="16" max="16" width="43.26953125" customWidth="1"/>
   </cols>
@@ -891,13 +946,21 @@
       <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
@@ -905,23 +968,35 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2">
+        <v>14</v>
+      </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="3"/>
+      <c r="O2" t="s">
+        <v>58</v>
+      </c>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="2"/>
+      <c r="C3" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
@@ -929,121 +1004,127 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="L3" s="2">
+        <v>4.45</v>
+      </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2">
-        <v>8640</v>
-      </c>
-      <c r="I4" s="2">
-        <v>172800</v>
-      </c>
-      <c r="J4" s="2">
-        <v>17280</v>
-      </c>
+      <c r="O3" t="s">
+        <v>112</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2">
+        <v>6.9809999999999997E-2</v>
+      </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s">
-        <v>58</v>
-      </c>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2">
-        <v>67500</v>
-      </c>
-      <c r="I5" s="2">
-        <v>82500</v>
-      </c>
-      <c r="J5" s="3"/>
+      <c r="C5" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="L5" s="3">
+        <v>7.6420000000000004E-5</v>
+      </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" t="s">
-        <v>58</v>
-      </c>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>62</v>
+      <c r="C6" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>70.67</v>
-      </c>
-      <c r="J6" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.99</v>
+      </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" t="s">
@@ -1052,71 +1133,74 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>62</v>
+      <c r="C7" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>205.33</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="J7" s="2">
+        <v>-4.75</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" t="s">
-        <v>58</v>
-      </c>
-      <c r="P7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>94</v>
+      <c r="C8" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2">
-        <v>1</v>
+      <c r="L8" s="3">
+        <v>100</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1126,217 +1210,232 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>57</v>
+      <c r="C9" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="I9" s="3">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="J9" s="2"/>
+      <c r="H9" s="2">
+        <v>8640</v>
+      </c>
+      <c r="I9" s="2">
+        <v>172800</v>
+      </c>
+      <c r="J9" s="2">
+        <v>17280</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
+      <c r="C10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="2">
-        <v>100</v>
-      </c>
+      <c r="H10" s="2">
+        <v>67500</v>
+      </c>
+      <c r="I10" s="2">
+        <v>82500</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>70.67</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>205.33</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" t="s">
+        <v>58</v>
+      </c>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" t="s">
         <v>63</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11">
-        <v>0.89</v>
-      </c>
-      <c r="I11">
-        <v>0.99</v>
-      </c>
-      <c r="J11">
-        <v>0.99</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="O11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12">
-        <v>0.1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="O12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13">
-        <v>0.18</v>
-      </c>
-      <c r="I13">
-        <v>0.97</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="O13" t="s">
-        <v>79</v>
-      </c>
+      <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>82</v>
+      <c r="B14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H14">
-        <v>0.49</v>
-      </c>
-      <c r="I14">
-        <v>0.99</v>
-      </c>
-      <c r="J14">
-        <v>0.99</v>
-      </c>
+      <c r="H14" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="I14" s="3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
       <c r="O14" t="s">
         <v>79</v>
       </c>
+      <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
@@ -1346,29 +1445,30 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>5</v>
+        <v>61</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H15">
-        <v>0.95</v>
-      </c>
-      <c r="I15">
-        <v>0.99</v>
-      </c>
-      <c r="K15" s="2"/>
+      <c r="L15" s="2">
+        <v>100</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
       <c r="O15" t="s">
-        <v>79</v>
+        <v>63</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -1379,26 +1479,30 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>83</v>
+        <v>66</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H16">
-        <v>5.7</v>
+        <v>0.89</v>
       </c>
       <c r="I16">
-        <v>6.2</v>
-      </c>
+        <v>0.99</v>
+      </c>
+      <c r="J16">
+        <v>0.99</v>
+      </c>
+      <c r="K16" s="2"/>
       <c r="O16" t="s">
         <v>79</v>
       </c>
@@ -1411,12 +1515,12 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>82</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -1426,33 +1530,34 @@
         <v>25</v>
       </c>
       <c r="H17">
-        <v>0.84</v>
+        <v>0.1</v>
       </c>
       <c r="I17">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>0.99</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K17" s="2"/>
       <c r="O17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>39</v>
+      <c r="A18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>5</v>
@@ -1460,121 +1565,101 @@
       <c r="G18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="2">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="I18" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="J18" s="3"/>
+      <c r="H18">
+        <v>0.18</v>
+      </c>
+      <c r="I18">
+        <v>0.97</v>
+      </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
       <c r="O18" t="s">
-        <v>40</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>43</v>
+      <c r="A19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>0.49</v>
+      </c>
+      <c r="I19">
+        <v>0.99</v>
+      </c>
+      <c r="J19">
+        <v>0.99</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="O19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="2">
-        <v>21</v>
-      </c>
-      <c r="I19" s="2">
-        <v>28</v>
-      </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" t="s">
-        <v>44</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="2">
-        <v>17.32</v>
-      </c>
-      <c r="I20" s="3">
-        <v>25.38</v>
-      </c>
-      <c r="J20" s="3">
-        <v>22.73</v>
+      <c r="H20">
+        <v>0.95</v>
+      </c>
+      <c r="I20">
+        <v>0.99</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
       <c r="O20" t="s">
-        <v>46</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>52</v>
+      <c r="A21" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>5</v>
@@ -1582,104 +1667,311 @@
       <c r="G21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21">
+        <v>5.7</v>
+      </c>
+      <c r="I21">
+        <v>6.2</v>
+      </c>
+      <c r="O21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22">
+        <v>0.84</v>
+      </c>
+      <c r="I22">
+        <v>0.99</v>
+      </c>
+      <c r="J22">
+        <v>0.99</v>
+      </c>
+      <c r="O22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" t="s">
+        <v>40</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="2">
+        <v>21</v>
+      </c>
+      <c r="I24" s="2">
+        <v>28</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="2">
+        <v>17.32</v>
+      </c>
+      <c r="I25" s="3">
+        <v>25.38</v>
+      </c>
+      <c r="J25" s="3">
+        <v>22.73</v>
+      </c>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" t="s">
+        <v>46</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="3">
         <v>0.26</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I26" s="3">
         <v>0.31</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" t="s">
+      <c r="J26" s="3"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" t="s">
         <v>50</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="P26" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B27" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C27" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D27" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E27" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="3">
+      <c r="G27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="3">
         <v>0.5</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I27" s="3">
         <v>1</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" t="s">
+      <c r="J27" s="3"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" t="s">
         <v>55</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="P27" s="2" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="721" yWindow="594" count="8">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K11:K15">
-      <formula1>I11</formula1>
-      <formula2>J11</formula2>
+  <dataValidations xWindow="721" yWindow="594" count="10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K16:K20">
+      <formula1>I16</formula1>
+      <formula2>J16</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L18:L22 L2:L9"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J18:J22 J2:J9">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L23:L27 L2:L6 L8:L14"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J23:J27 J2:J14">
       <formula1>H2</formula1>
       <formula2>I2</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M18:M22 M2:M9"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N18:N22 N2:N9"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K18:K22 K2:K9">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M23:M27 M2:M14"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N23:N27 N2:N14"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K23:K27 K2:K14">
       <formula1>I2</formula1>
       <formula2>J2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I18:I22 I2:I9">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I23:I27 I2:I6 I8:I14">
       <formula1>H2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H18:H22 H2:H9">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H23:H27 H2:H6 H8:H14">
       <formula1>I2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="L7">
+      <formula1>H7</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H7">
+      <formula1>L7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="721" yWindow="594" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="721" yWindow="594" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
           <x14:formula1>
             <xm:f>ListItem!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F11:F22 F9 F2:F7</xm:sqref>
+          <xm:sqref>F16:F27 F14 F9:F12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Truncated" prompt="Is the probability distribution truncated?">
           <x14:formula1>
             <xm:f>ListItem!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G22</xm:sqref>
+          <xm:sqref>G2:G27</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
+          <x14:formula1>
+            <xm:f>ListItem!$A$2:$A$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>F7 F6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>ListItem!$A$2:$A$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>F5 F4 F3 F2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1692,7 +1984,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1819,7 +2111,9 @@
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>

</xml_diff>

<commit_message>
computation of watershed conc.
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="134">
   <si>
     <t>Variable</t>
   </si>
@@ -391,13 +391,58 @@
   </si>
   <si>
     <t>LogNormal3</t>
+  </si>
+  <si>
+    <t>kg/m²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manure application rate </t>
+  </si>
+  <si>
+    <t>Fraction of manure that runs off</t>
+  </si>
+  <si>
+    <t>Fraction of E.coli surviving transport</t>
+  </si>
+  <si>
+    <t>Surface area of the waterbody</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>Average depth of the waterbody</t>
+  </si>
+  <si>
+    <t>Conversion factor from kg to g</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w_area </t>
+  </si>
+  <si>
+    <t xml:space="preserve">runoff </t>
+  </si>
+  <si>
+    <t xml:space="preserve">transport </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c_factor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">m_apply </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,8 +482,22 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +564,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -527,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -549,6 +620,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1912,6 +1986,180 @@
       </c>
       <c r="P27" s="2" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28">
+        <v>10</v>
+      </c>
+      <c r="O28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L29">
+        <v>0.1</v>
+      </c>
+      <c r="O29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30">
+        <v>0.5</v>
+      </c>
+      <c r="O30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31">
+        <v>10000</v>
+      </c>
+      <c r="O31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="O32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A33" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33">
+        <v>1000000</v>
+      </c>
+      <c r="O33" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1959,19 +2207,19 @@
           <x14:formula1>
             <xm:f>ListItem!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G27</xm:sqref>
+          <xm:sqref>G2:G33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
           <x14:formula1>
             <xm:f>ListItem!$A$2:$A$17</xm:f>
           </x14:formula1>
-          <xm:sqref>F7 F6</xm:sqref>
+          <xm:sqref>F6:F7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ListItem!$A$2:$A$17</xm:f>
           </x14:formula1>
-          <xm:sqref>F5 F4 F3 F2</xm:sqref>
+          <xm:sqref>F2:F5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>